<commit_message>
handles voucher and refunds tabs
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -2090,11 +2090,6 @@
           <t>USD</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>https://www.virtualelvisweek.com/legacy/index.html</t>
-        </is>
-      </c>
       <c r="I26" t="inlineStr">
         <is>
           <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
@@ -2150,11 +2145,6 @@
       <c r="F27" t="inlineStr">
         <is>
           <t>USD</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>https://virtualelvisweek.com/superfan/index.html</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -4668,7 +4658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4770,6 +4760,2106 @@
       <c r="S1" t="inlineStr">
         <is>
           <t>Payment Tool Token</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TRX-0055</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>55</v>
+      </c>
+      <c r="K2" t="n">
+        <v>55</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>100</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>7/7/22 20:39</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRX-0048</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>48</v>
+      </c>
+      <c r="K3" t="n">
+        <v>48</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>100</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>7/7/22 19:02</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TRX-0046</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>46</v>
+      </c>
+      <c r="K4" t="n">
+        <v>46</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>100</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>7/7/22 18:19</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TRX-0041</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>41</v>
+      </c>
+      <c r="K5" t="n">
+        <v>41</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>100</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>7/7/22 17:45</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TRX-0040</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>40</v>
+      </c>
+      <c r="K6" t="n">
+        <v>40</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>100</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>7/7/22 17:40</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TRX-0026</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>26</v>
+      </c>
+      <c r="K7" t="n">
+        <v>26</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>100</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>7/6/22 18:53</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TRX-0025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>25</v>
+      </c>
+      <c r="K8" t="n">
+        <v>25</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>100</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>7/6/22 18:16</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TRX-0024</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>24</v>
+      </c>
+      <c r="K9" t="n">
+        <v>24</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>100</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>7/6/22 18:05</t>
+        </is>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TRX-0023</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>23</v>
+      </c>
+      <c r="K10" t="n">
+        <v>23</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>100</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>7/6/22 18:04</t>
+        </is>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TRX-0022</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>22</v>
+      </c>
+      <c r="K11" t="n">
+        <v>22</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>100</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>7/6/22 18:02</t>
+        </is>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TRX-0021</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>21</v>
+      </c>
+      <c r="K12" t="n">
+        <v>21</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>100</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>7/6/22 17:58</t>
+        </is>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TRX-0020</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>20</v>
+      </c>
+      <c r="K13" t="n">
+        <v>20</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>100</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>7/6/22 17:56</t>
+        </is>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TRX-0019</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>19</v>
+      </c>
+      <c r="K14" t="n">
+        <v>19</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>100</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>7/6/22 17:53</t>
+        </is>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TRX-0018</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>18</v>
+      </c>
+      <c r="K15" t="n">
+        <v>18</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>100</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>7/6/22 17:51</t>
+        </is>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TRX-0017</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>17</v>
+      </c>
+      <c r="K16" t="n">
+        <v>17</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>100</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>7/6/22 17:51</t>
+        </is>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TRX-0016</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>16</v>
+      </c>
+      <c r="K17" t="n">
+        <v>16</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>100</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>7/6/22 17:49</t>
+        </is>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TRX-0015</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>15</v>
+      </c>
+      <c r="K18" t="n">
+        <v>15</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>100</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>7/6/22 17:15</t>
+        </is>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TRX-0014</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>14</v>
+      </c>
+      <c r="K19" t="n">
+        <v>14</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>100</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>7/6/22 17:09</t>
+        </is>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TRX-0013</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>13</v>
+      </c>
+      <c r="K20" t="n">
+        <v>13</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>100</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>7/6/22 16:54</t>
+        </is>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>TRX-0012</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>12</v>
+      </c>
+      <c r="K21" t="n">
+        <v>12</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>100</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>7/6/22 16:50</t>
+        </is>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>TRX-0011</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>11</v>
+      </c>
+      <c r="K22" t="n">
+        <v>11</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>100</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>7/6/22 16:38</t>
+        </is>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TRX-0010</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>10</v>
+      </c>
+      <c r="K23" t="n">
+        <v>10</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>100</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>7/6/22 16:08</t>
+        </is>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TRX-0009</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>9</v>
+      </c>
+      <c r="K24" t="n">
+        <v>9</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>100</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>7/6/22 15:33</t>
+        </is>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>TRX-0008</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>8</v>
+      </c>
+      <c r="K25" t="n">
+        <v>8</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>100</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>7/6/22 15:30</t>
+        </is>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TRX-0007</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>7</v>
+      </c>
+      <c r="K26" t="n">
+        <v>7</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>100</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>7/6/22 13:44</t>
+        </is>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>TRX-0006</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>6</v>
+      </c>
+      <c r="K27" t="n">
+        <v>6</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>100</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>7/6/22 4:41</t>
+        </is>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>TRX-0005</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>5</v>
+      </c>
+      <c r="K28" t="n">
+        <v>5</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>100</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>7/6/22 4:38</t>
+        </is>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>TRX-0004</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>4</v>
+      </c>
+      <c r="K29" t="n">
+        <v>4</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>100</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>7/5/22 21:31</t>
+        </is>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>TRX-0003</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3127729</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Elvis Week Tribute Artist Pass</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Elvis Week Tribute Pass- 4 Live Tribute Pass Events + 1 Week  VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>3</v>
+      </c>
+      <c r="K30" t="n">
+        <v>3</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>100</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>7/5/22 21:30</t>
+        </is>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>TRX-0002</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Used voucher VoucherName (voucherCode),</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>2</v>
+      </c>
+      <c r="K31" t="n">
+        <v>2</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>100</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>7/5/22 20:45</t>
+        </is>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>voucherCode</t>
         </is>
       </c>
     </row>
@@ -4784,7 +6874,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4889,6 +6979,120 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TRX-0033</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>3127710</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>132</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Elvis Week Legacy Pass- 5 Live Legacy Pass Events + 1 Week VOD Each - $130 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>33</v>
+      </c>
+      <c r="K2" t="n">
+        <v>33</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>7/7/22 16:47</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>ch_</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRX-0032</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3177496</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>package</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Elvis Super Fan Package</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>227</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Elvis Week Super Fan- All 9 Live Events + 7 Days VOD Each+ Graceland Mansion Virtual Tour!- + 72 Hours VOD Each - $225 + $2 Processing Fee</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>32</v>
+      </c>
+      <c r="K3" t="n">
+        <v>32</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>7/7/22 16:46</t>
+        </is>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>ch_</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>